<commit_message>
Added two more test cases
</commit_message>
<xml_diff>
--- a/Test Cases/Test Cases.xlsx
+++ b/Test Cases/Test Cases.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Sr No</t>
   </si>
@@ -35,6 +35,32 @@
 4)I agree terms &amp; condition default to Yes
 5)SIGN UP button
 6)Link to existing Login process</t>
+  </si>
+  <si>
+    <t>Assigned To</t>
+  </si>
+  <si>
+    <t>TC2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Website  should display Trending tags on search </t>
+  </si>
+  <si>
+    <t>TC3</t>
+  </si>
+  <si>
+    <t>Rahul</t>
+  </si>
+  <si>
+    <t>Satish</t>
+  </si>
+  <si>
+    <t>When customer click  search button and select any trending tags then 
+1) Flat offer pop up should be displayed
+2) customer is asked to specify if its for Girl or a boy
+3) customer must be given option of Tiny preemie, Preemie and 0-3M 3-5M,6-9M and +More
+4) Apply button is available
+5) When customer complete step 2-4 then min 5 products are displayed</t>
   </si>
 </sst>
 </file>
@@ -386,19 +412,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I14:I15"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="34.7109375" customWidth="1"/>
+    <col min="3" max="3" width="49" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -408,8 +435,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -418,6 +448,37 @@
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>